<commit_message>
modify projects 2 & 3 data with @rubenalv
</commit_message>
<xml_diff>
--- a/data/20170201_GEP00003/20170201_GEP00003.xlsx
+++ b/data/20170201_GEP00003/20170201_GEP00003.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="213">
   <si>
     <t xml:space="preserve">geid</t>
   </si>
@@ -99,6 +99,15 @@
   </si>
   <si>
     <t xml:space="preserve">GFP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRCm38.p5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">forward</t>
   </si>
   <si>
     <t xml:space="preserve">&gt;Full eGFP coding sequence: ATGGTGAGCAAGGGCGAGGAGCTGTTCACCGGGGTGGTGCCCATCCTGGTCGAGCTGGACGGCGACGTAAACGGCCACAAGTTCAGCGTGTCCGGCGAGGGCGAGGGCGATGCCACCTACGGCAAGCTGACCCTGAAGTTCATCTGCACCACCGGCAAGCTGCCCGTGCCCTGGCCCACCCTCGTGACCACCCTGACCTACGGCGTGCAGTGCTTCAGCCGCTACCCCGACCACATGAAGCAGCACGACTTCTTCAAGTCCGCCATGCCCGAAGGCTACGTCCAGGAGCGCACCATCTTCTTCAAGGACGACGGCAACTACAAGACCCGCGCCGAGGTGAAGTTCGAGGGCGACACCCTGGTGAACCGCATCGAGCTGAAGGGCATCGACTTCAAGGAGGACGGCAACATCCTGGGGCACAAGCTGGAGTACAACTACAACAGCCACAACGTCTATATCATGGCCGACAAGCAGAAGAACGGCATCAAGGTGAACTTCAAGATCCGCCACAACATCGAGGACGGCAGCGTGCAGCTCGCCGACCACTACCAGCAGAACACCCCCATCGGCGACGGCCCCGTGCTGCTGCCCGACAACCACTACCTGAGCACCCAGTCCGCCCTGAGCAAAGACCCCAACGAGAAGCGCGATCACATGGTCCTGCTGGAGTTCGTGACCGCCGCCGGGATCACTCTCGGCATGGACGAGCTGTACAAGTAA</t>
@@ -668,7 +677,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -709,11 +718,6 @@
       <name val="Calibri;sans-serif"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -764,7 +768,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -790,10 +794,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -890,7 +890,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.28"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="15.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="15.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="33.8"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
   </cols>
@@ -966,7 +966,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1017,8 +1017,29 @@
       <c r="B2" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="C2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>26</v>
+      </c>
       <c r="J2" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1045,34 +1066,34 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.62"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1080,22 +1101,22 @@
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>62</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1123,22 +1144,22 @@
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.95"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1157,10 +1178,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O11" activeCellId="0" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1186,52 +1207,52 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="Q1" s="0" t="s">
         <v>7</v>
@@ -1239,39 +1260,27 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F2" s="5"/>
       <c r="I2" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="F3" s="5"/>
-      <c r="J3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="8"/>
+        <v>61</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>62</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1292,7 +1301,7 @@
   <dimension ref="A1:J97"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B62" activeCellId="0" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1302,7 +1311,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
   </cols>
@@ -1312,28 +1321,28 @@
         <v>15</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1341,22 +1350,22 @@
         <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="H2" s="8"/>
+        <v>71</v>
+      </c>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1364,10 +1373,10 @@
         <v>8</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1375,10 +1384,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1386,10 +1395,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1397,10 +1406,10 @@
         <v>8</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1408,10 +1417,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1419,10 +1428,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1430,10 +1439,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1441,10 +1450,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1452,10 +1461,10 @@
         <v>8</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1463,10 +1472,10 @@
         <v>8</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1474,10 +1483,10 @@
         <v>8</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1485,10 +1494,10 @@
         <v>8</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1496,10 +1505,10 @@
         <v>8</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1507,10 +1516,10 @@
         <v>8</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1518,94 +1527,94 @@
         <v>8</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="H18" s="8"/>
+        <v>87</v>
+      </c>
+      <c r="H18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="H19" s="8"/>
+        <v>88</v>
+      </c>
+      <c r="H19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="H20" s="8"/>
+        <v>89</v>
+      </c>
+      <c r="H20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="H21" s="8"/>
+        <v>90</v>
+      </c>
+      <c r="H21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="H22" s="8"/>
+        <v>91</v>
+      </c>
+      <c r="H22" s="7"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="H23" s="8"/>
+        <v>92</v>
+      </c>
+      <c r="H23" s="7"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="H24" s="8"/>
+        <v>93</v>
+      </c>
+      <c r="H24" s="7"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1613,10 +1622,10 @@
         <v>8</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1624,130 +1633,130 @@
         <v>8</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="H27" s="8"/>
+        <v>96</v>
+      </c>
+      <c r="H27" s="7"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="H28" s="8"/>
+        <v>97</v>
+      </c>
+      <c r="H28" s="7"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="H29" s="8"/>
+        <v>98</v>
+      </c>
+      <c r="H29" s="7"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="H30" s="8"/>
+        <v>99</v>
+      </c>
+      <c r="H30" s="7"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="H31" s="8"/>
+        <v>100</v>
+      </c>
+      <c r="H31" s="7"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="H32" s="8"/>
+        <v>101</v>
+      </c>
+      <c r="H32" s="7"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="H33" s="8"/>
+        <v>102</v>
+      </c>
+      <c r="H33" s="7"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="H34" s="8"/>
+        <v>103</v>
+      </c>
+      <c r="H34" s="7"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="H35" s="8"/>
+        <v>104</v>
+      </c>
+      <c r="H35" s="7"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="H36" s="8"/>
+        <v>105</v>
+      </c>
+      <c r="H36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1755,10 +1764,10 @@
         <v>8</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1766,130 +1775,130 @@
         <v>8</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="H39" s="8"/>
+        <v>108</v>
+      </c>
+      <c r="H39" s="7"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="H40" s="8"/>
+        <v>109</v>
+      </c>
+      <c r="H40" s="7"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="H41" s="8"/>
+        <v>110</v>
+      </c>
+      <c r="H41" s="7"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="H42" s="8"/>
+        <v>111</v>
+      </c>
+      <c r="H42" s="7"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="H43" s="8"/>
+        <v>112</v>
+      </c>
+      <c r="H43" s="7"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="H44" s="8"/>
+        <v>113</v>
+      </c>
+      <c r="H44" s="7"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="H45" s="8"/>
+        <v>114</v>
+      </c>
+      <c r="H45" s="7"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="H46" s="8"/>
+        <v>115</v>
+      </c>
+      <c r="H46" s="7"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="H47" s="8"/>
+        <v>116</v>
+      </c>
+      <c r="H47" s="7"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="H48" s="8"/>
+        <v>117</v>
+      </c>
+      <c r="H48" s="7"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1897,10 +1906,10 @@
         <v>8</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1908,130 +1917,130 @@
         <v>8</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="H51" s="8"/>
+        <v>120</v>
+      </c>
+      <c r="H51" s="7"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="H52" s="8"/>
+        <v>121</v>
+      </c>
+      <c r="H52" s="7"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="H53" s="8"/>
+        <v>122</v>
+      </c>
+      <c r="H53" s="7"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="H54" s="8"/>
+        <v>123</v>
+      </c>
+      <c r="H54" s="7"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="H55" s="8"/>
+        <v>124</v>
+      </c>
+      <c r="H55" s="7"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="H56" s="8"/>
+        <v>125</v>
+      </c>
+      <c r="H56" s="7"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="H57" s="8"/>
+        <v>126</v>
+      </c>
+      <c r="H57" s="7"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="H58" s="8"/>
+        <v>127</v>
+      </c>
+      <c r="H58" s="7"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="H59" s="8"/>
+        <v>128</v>
+      </c>
+      <c r="H59" s="7"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="H60" s="8"/>
+        <v>129</v>
+      </c>
+      <c r="H60" s="7"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2039,31 +2048,31 @@
         <v>8</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="G62" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H62" s="8" t="n">
+      <c r="H62" s="7" t="n">
         <v>0</v>
       </c>
       <c r="I62" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2071,29 +2080,29 @@
         <v>8</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="G63" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="H63" s="8" t="n">
+      <c r="H63" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="I63" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2101,29 +2110,29 @@
         <v>8</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="G64" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="H64" s="8" t="n">
+      <c r="H64" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="I64" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2131,29 +2140,29 @@
         <v>8</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="G65" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="H65" s="8" t="n">
+      <c r="H65" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="I65" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2161,29 +2170,29 @@
         <v>8</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G66" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="H66" s="8" t="n">
+      <c r="H66" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="I66" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2191,29 +2200,29 @@
         <v>8</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="G67" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="H67" s="8" t="n">
+      <c r="H67" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="I67" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2221,29 +2230,29 @@
         <v>8</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="G68" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="H68" s="8" t="n">
+      <c r="H68" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="I68" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2251,29 +2260,29 @@
         <v>8</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="G69" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="H69" s="8" t="n">
+      <c r="H69" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="I69" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2281,29 +2290,29 @@
         <v>8</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="G70" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="H70" s="8" t="n">
+      <c r="H70" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="I70" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2311,29 +2320,29 @@
         <v>8</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="G71" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="H71" s="8" t="n">
+      <c r="H71" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="I71" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2341,26 +2350,26 @@
         <v>8</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="G72" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="H72" s="8" t="n">
+      <c r="H72" s="7" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="I72" s="0" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2368,10 +2377,10 @@
         <v>8</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2379,10 +2388,10 @@
         <v>8</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2390,130 +2399,130 @@
         <v>8</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="H75" s="8"/>
+        <v>157</v>
+      </c>
+      <c r="H75" s="7"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="H76" s="8"/>
+        <v>158</v>
+      </c>
+      <c r="H76" s="7"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="H77" s="8"/>
+        <v>159</v>
+      </c>
+      <c r="H77" s="7"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="H78" s="8"/>
+        <v>160</v>
+      </c>
+      <c r="H78" s="7"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="H79" s="8"/>
+        <v>161</v>
+      </c>
+      <c r="H79" s="7"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="H80" s="8"/>
+        <v>162</v>
+      </c>
+      <c r="H80" s="7"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="H81" s="8"/>
+        <v>163</v>
+      </c>
+      <c r="H81" s="7"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="H82" s="8"/>
+        <v>164</v>
+      </c>
+      <c r="H82" s="7"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="H83" s="8"/>
+        <v>165</v>
+      </c>
+      <c r="H83" s="7"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="H84" s="8"/>
+        <v>166</v>
+      </c>
+      <c r="H84" s="7"/>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2521,10 +2530,10 @@
         <v>8</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2532,10 +2541,10 @@
         <v>8</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2543,10 +2552,10 @@
         <v>8</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2554,10 +2563,10 @@
         <v>8</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2565,10 +2574,10 @@
         <v>8</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2576,10 +2585,10 @@
         <v>8</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2587,10 +2596,10 @@
         <v>8</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2598,10 +2607,10 @@
         <v>8</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2609,10 +2618,10 @@
         <v>8</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2620,10 +2629,10 @@
         <v>8</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2631,10 +2640,10 @@
         <v>8</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2642,12 +2651,12 @@
         <v>8</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="H97" s="8"/>
+        <v>179</v>
+      </c>
+      <c r="H97" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2675,16 +2684,16 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="73.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="73.09"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>0</v>
@@ -2711,8 +2720,8 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2727,314 +2736,314 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>10</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>11</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>12</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>13</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>14</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>15</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>16</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>17</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>18</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>19</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>20</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated GEP00003 with guide and primer locations relative to GFP and Plate ids
</commit_message>
<xml_diff>
--- a/data/20170201_GEP00003/20170201_GEP00003.xlsx
+++ b/data/20170201_GEP00003/20170201_GEP00003.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="219">
   <si>
     <t xml:space="preserve">geid</t>
   </si>
@@ -71,7 +71,7 @@
     <t xml:space="preserve">Alasdair Russel</t>
   </si>
   <si>
-    <t xml:space="preserve">eGFP Knock-in to turn it into eBFP</t>
+    <t xml:space="preserve">eGFP Knock-in to turn it into eBFP. NGS to detect the modification in a population of cells.</t>
   </si>
   <si>
     <t xml:space="preserve">project_geid</t>
@@ -203,6 +203,18 @@
     <t xml:space="preserve">Knock-in</t>
   </si>
   <si>
+    <t xml:space="preserve">reverse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gene</t>
+  </si>
+  <si>
     <t xml:space="preserve">RA25_235</t>
   </si>
   <si>
@@ -215,7 +227,7 @@
     <t xml:space="preserve">GGCGGACTTGAAGAAGTCGT</t>
   </si>
   <si>
-    <t xml:space="preserve">NGS_GFPtoBFB-F NGS_GFPtoBFP-R</t>
+    <t xml:space="preserve">primer locations relative to GFP coding sequence</t>
   </si>
   <si>
     <t xml:space="preserve">layout_geid</t>
@@ -573,6 +585,12 @@
   </si>
   <si>
     <t xml:space="preserve">plate_barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GEP00003_01_NGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shared SLX-13774 wth GEP00002</t>
   </si>
   <si>
     <t xml:space="preserve">dna_source</t>
@@ -789,7 +807,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -880,19 +898,19 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.28"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="15.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="33.8"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="33.4795918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -950,7 +968,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -965,17 +983,17 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.54"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.28"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1045,7 +1063,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1060,17 +1078,17 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.62"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.6989795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1112,6 +1130,9 @@
       <c r="E2" s="0" t="n">
         <v>62</v>
       </c>
+      <c r="F2" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="G2" s="0" t="s">
         <v>37</v>
       </c>
@@ -1122,7 +1143,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1137,15 +1158,15 @@
   </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.95"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.6224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1165,7 +1186,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1180,29 +1201,30 @@
   </sheetPr>
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O11" activeCellId="0" sqref="O11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.92"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="28.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="14.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="14.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="31.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="31.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="18" style="0" width="14.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="10.27"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="22" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.66836734693878"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.9438775510204"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="26.2602040816327"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.2704081632653"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.1989795918367"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="20" min="18" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1265,27 +1287,56 @@
       <c r="B2" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="C2" s="0" t="n">
+        <v>202</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="I2" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>59</v>
+        <v>63</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>131</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>151</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>61</v>
+        <v>65</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>245</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <v>264</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -1300,20 +1351,20 @@
   </sheetPr>
   <dimension ref="A1:J97"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B62" activeCellId="0" sqref="B62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="20.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1321,28 +1372,28 @@
         <v>15</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>39</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1350,10 +1401,10 @@
         <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="H2" s="7"/>
     </row>
@@ -1362,10 +1413,10 @@
         <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1373,10 +1424,10 @@
         <v>8</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1384,10 +1435,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1395,10 +1446,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1406,10 +1457,10 @@
         <v>8</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1417,10 +1468,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1428,10 +1479,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1439,10 +1490,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1450,10 +1501,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1461,10 +1512,10 @@
         <v>8</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1472,10 +1523,10 @@
         <v>8</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1483,10 +1534,10 @@
         <v>8</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1494,10 +1545,10 @@
         <v>8</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1505,10 +1556,10 @@
         <v>8</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1516,10 +1567,10 @@
         <v>8</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1527,10 +1578,10 @@
         <v>8</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="H18" s="7"/>
     </row>
@@ -1539,10 +1590,10 @@
         <v>8</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="H19" s="7"/>
     </row>
@@ -1551,10 +1602,10 @@
         <v>8</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="H20" s="7"/>
     </row>
@@ -1563,10 +1614,10 @@
         <v>8</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="H21" s="7"/>
     </row>
@@ -1575,10 +1626,10 @@
         <v>8</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="H22" s="7"/>
     </row>
@@ -1587,10 +1638,10 @@
         <v>8</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="H23" s="7"/>
     </row>
@@ -1599,10 +1650,10 @@
         <v>8</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H24" s="7"/>
     </row>
@@ -1611,10 +1662,10 @@
         <v>8</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1622,10 +1673,10 @@
         <v>8</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1633,10 +1684,10 @@
         <v>8</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="H27" s="7"/>
     </row>
@@ -1645,10 +1696,10 @@
         <v>8</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="H28" s="7"/>
     </row>
@@ -1657,10 +1708,10 @@
         <v>8</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="H29" s="7"/>
     </row>
@@ -1669,10 +1720,10 @@
         <v>8</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="H30" s="7"/>
     </row>
@@ -1681,10 +1732,10 @@
         <v>8</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="H31" s="7"/>
     </row>
@@ -1693,10 +1744,10 @@
         <v>8</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="H32" s="7"/>
     </row>
@@ -1705,10 +1756,10 @@
         <v>8</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="H33" s="7"/>
     </row>
@@ -1717,10 +1768,10 @@
         <v>8</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="H34" s="7"/>
     </row>
@@ -1729,10 +1780,10 @@
         <v>8</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="H35" s="7"/>
     </row>
@@ -1741,10 +1792,10 @@
         <v>8</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="H36" s="7"/>
     </row>
@@ -1753,10 +1804,10 @@
         <v>8</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1764,10 +1815,10 @@
         <v>8</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1775,10 +1826,10 @@
         <v>8</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="H39" s="7"/>
     </row>
@@ -1787,10 +1838,10 @@
         <v>8</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="H40" s="7"/>
     </row>
@@ -1799,10 +1850,10 @@
         <v>8</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="H41" s="7"/>
     </row>
@@ -1811,10 +1862,10 @@
         <v>8</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="H42" s="7"/>
     </row>
@@ -1823,10 +1874,10 @@
         <v>8</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H43" s="7"/>
     </row>
@@ -1835,10 +1886,10 @@
         <v>8</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="H44" s="7"/>
     </row>
@@ -1847,10 +1898,10 @@
         <v>8</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="H45" s="7"/>
     </row>
@@ -1859,10 +1910,10 @@
         <v>8</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="H46" s="7"/>
     </row>
@@ -1871,10 +1922,10 @@
         <v>8</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="H47" s="7"/>
     </row>
@@ -1883,10 +1934,10 @@
         <v>8</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="H48" s="7"/>
     </row>
@@ -1895,10 +1946,10 @@
         <v>8</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1906,10 +1957,10 @@
         <v>8</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1917,10 +1968,10 @@
         <v>8</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="H51" s="7"/>
     </row>
@@ -1929,10 +1980,10 @@
         <v>8</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H52" s="7"/>
     </row>
@@ -1941,10 +1992,10 @@
         <v>8</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="H53" s="7"/>
     </row>
@@ -1953,10 +2004,10 @@
         <v>8</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="H54" s="7"/>
     </row>
@@ -1965,10 +2016,10 @@
         <v>8</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="H55" s="7"/>
     </row>
@@ -1977,10 +2028,10 @@
         <v>8</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="H56" s="7"/>
     </row>
@@ -1989,10 +2040,10 @@
         <v>8</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="H57" s="7"/>
     </row>
@@ -2001,10 +2052,10 @@
         <v>8</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="H58" s="7"/>
     </row>
@@ -2013,10 +2064,10 @@
         <v>8</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="H59" s="7"/>
     </row>
@@ -2025,10 +2076,10 @@
         <v>8</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="H60" s="7"/>
     </row>
@@ -2037,10 +2088,10 @@
         <v>8</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2048,19 +2099,19 @@
         <v>8</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="G62" s="0" t="n">
         <v>1</v>
@@ -2069,10 +2120,10 @@
         <v>0</v>
       </c>
       <c r="I62" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2080,19 +2131,19 @@
         <v>8</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C63" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="E63" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="D63" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="E63" s="0" t="s">
-        <v>133</v>
-      </c>
       <c r="F63" s="4" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="G63" s="0" t="n">
         <v>2</v>
@@ -2102,7 +2153,7 @@
         <v>0</v>
       </c>
       <c r="I63" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2110,19 +2161,19 @@
         <v>8</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="G64" s="0" t="n">
         <v>3</v>
@@ -2132,7 +2183,7 @@
         <v>0</v>
       </c>
       <c r="I64" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2140,19 +2191,19 @@
         <v>8</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="G65" s="0" t="n">
         <v>4</v>
@@ -2162,7 +2213,7 @@
         <v>0</v>
       </c>
       <c r="I65" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2170,19 +2221,19 @@
         <v>8</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="G66" s="0" t="n">
         <v>5</v>
@@ -2192,7 +2243,7 @@
         <v>0</v>
       </c>
       <c r="I66" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2200,19 +2251,19 @@
         <v>8</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="G67" s="0" t="n">
         <v>6</v>
@@ -2222,7 +2273,7 @@
         <v>0</v>
       </c>
       <c r="I67" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2230,19 +2281,19 @@
         <v>8</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="G68" s="0" t="n">
         <v>7</v>
@@ -2252,7 +2303,7 @@
         <v>0</v>
       </c>
       <c r="I68" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2260,19 +2311,19 @@
         <v>8</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="G69" s="0" t="n">
         <v>8</v>
@@ -2282,7 +2333,7 @@
         <v>0</v>
       </c>
       <c r="I69" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2290,19 +2341,19 @@
         <v>8</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="G70" s="0" t="n">
         <v>9</v>
@@ -2312,7 +2363,7 @@
         <v>0</v>
       </c>
       <c r="I70" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2320,19 +2371,19 @@
         <v>8</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="G71" s="0" t="n">
         <v>10</v>
@@ -2342,7 +2393,7 @@
         <v>0</v>
       </c>
       <c r="I71" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2350,16 +2401,16 @@
         <v>8</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="G72" s="0" t="n">
         <v>11</v>
@@ -2369,7 +2420,7 @@
         <v>1</v>
       </c>
       <c r="I72" s="0" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2377,10 +2428,10 @@
         <v>8</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2388,10 +2439,10 @@
         <v>8</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2399,10 +2450,10 @@
         <v>8</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="H75" s="7"/>
     </row>
@@ -2411,10 +2462,10 @@
         <v>8</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="H76" s="7"/>
     </row>
@@ -2423,10 +2474,10 @@
         <v>8</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="H77" s="7"/>
     </row>
@@ -2435,10 +2486,10 @@
         <v>8</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="H78" s="7"/>
     </row>
@@ -2447,10 +2498,10 @@
         <v>8</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H79" s="7"/>
     </row>
@@ -2459,10 +2510,10 @@
         <v>8</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="H80" s="7"/>
     </row>
@@ -2471,10 +2522,10 @@
         <v>8</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="H81" s="7"/>
     </row>
@@ -2483,10 +2534,10 @@
         <v>8</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="H82" s="7"/>
     </row>
@@ -2495,10 +2546,10 @@
         <v>8</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="H83" s="7"/>
     </row>
@@ -2507,10 +2558,10 @@
         <v>8</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="H84" s="7"/>
     </row>
@@ -2519,10 +2570,10 @@
         <v>8</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2530,10 +2581,10 @@
         <v>8</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2541,10 +2592,10 @@
         <v>8</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2552,10 +2603,10 @@
         <v>8</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2563,10 +2614,10 @@
         <v>8</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2574,10 +2625,10 @@
         <v>8</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2585,10 +2636,10 @@
         <v>8</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2596,10 +2647,10 @@
         <v>8</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2607,10 +2658,10 @@
         <v>8</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2618,10 +2669,10 @@
         <v>8</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2629,10 +2680,10 @@
         <v>8</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2640,10 +2691,10 @@
         <v>8</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2651,17 +2702,17 @@
         <v>8</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="H97" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2674,38 +2725,52 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="73.09"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="72.3571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2720,336 +2785,336 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="13.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="31.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>10</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
update model: new guide_mismatch table, new columns in project and mutation_summary tables; add loader for guide_mismatch
</commit_message>
<xml_diff>
--- a/data/20170201_GEP00003/20170201_GEP00003.xlsx
+++ b/data/20170201_GEP00003/20170201_GEP00003.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" state="visible" r:id="rId2"/>
@@ -38,7 +38,7 @@
     <t xml:space="preserve">scientist</t>
   </si>
   <si>
-    <t xml:space="preserve">institute</t>
+    <t xml:space="preserve">affiliation</t>
   </si>
   <si>
     <t xml:space="preserve">group</t>
@@ -152,10 +152,10 @@
     <t xml:space="preserve">is_off_target_coding_region</t>
   </si>
   <si>
-    <t xml:space="preserve">regions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mismatches</t>
+    <t xml:space="preserve">number_of_mismatches</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number_of_off_targets</t>
   </si>
   <si>
     <t xml:space="preserve">experiment_type</t>
@@ -236,6 +236,9 @@
     <t xml:space="preserve">cell_line_name</t>
   </si>
   <si>
+    <t xml:space="preserve">cell_pool</t>
+  </si>
+  <si>
     <t xml:space="preserve">clone_name</t>
   </si>
   <si>
@@ -573,9 +576,6 @@
   </si>
   <si>
     <t xml:space="preserve">library_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">barcode_size</t>
   </si>
   <si>
     <t xml:space="preserve">sequencing_barcode</t>
@@ -872,7 +872,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -957,7 +957,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+      <selection pane="topLeft" activeCell="J2" activeCellId="1" sqref="D1 J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1052,12 +1052,12 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="1" sqref="D1 F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.31"/>
@@ -1131,15 +1131,17 @@
   </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1175,15 +1177,15 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="1" sqref="D1 E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="11.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.61"/>
@@ -1322,10 +1324,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J97"/>
+  <dimension ref="A1:K97"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B44" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H55" activeCellId="0" sqref="H55"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="D1 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1333,11 +1335,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="20.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="11.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1357,10 +1359,10 @@
         <v>69</v>
       </c>
       <c r="F1" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>70</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>71</v>
@@ -1368,28 +1370,31 @@
       <c r="I1" s="0" t="s">
         <v>72</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="H2" s="7"/>
+        <v>75</v>
+      </c>
+      <c r="I2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1397,10 +1402,10 @@
         <v>8</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1408,10 +1413,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1419,10 +1424,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1430,10 +1435,10 @@
         <v>8</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1441,10 +1446,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1452,10 +1457,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1463,10 +1468,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1474,10 +1479,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1485,10 +1490,10 @@
         <v>8</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1496,10 +1501,10 @@
         <v>8</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1507,10 +1512,10 @@
         <v>8</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1518,10 +1523,10 @@
         <v>8</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1529,10 +1534,10 @@
         <v>8</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1540,10 +1545,10 @@
         <v>8</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1551,94 +1556,94 @@
         <v>8</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="H18" s="7"/>
+        <v>91</v>
+      </c>
+      <c r="I18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="H19" s="7"/>
+        <v>92</v>
+      </c>
+      <c r="I19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="H20" s="7"/>
+        <v>93</v>
+      </c>
+      <c r="I20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="H21" s="7"/>
+        <v>94</v>
+      </c>
+      <c r="I21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="H22" s="7"/>
+        <v>95</v>
+      </c>
+      <c r="I22" s="7"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="H23" s="7"/>
+        <v>96</v>
+      </c>
+      <c r="I23" s="7"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="H24" s="7"/>
+        <v>97</v>
+      </c>
+      <c r="I24" s="7"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1646,10 +1651,10 @@
         <v>8</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1657,130 +1662,130 @@
         <v>8</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="H27" s="7"/>
+        <v>100</v>
+      </c>
+      <c r="I27" s="7"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="H28" s="7"/>
+        <v>101</v>
+      </c>
+      <c r="I28" s="7"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="H29" s="7"/>
+        <v>102</v>
+      </c>
+      <c r="I29" s="7"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="H30" s="7"/>
+        <v>103</v>
+      </c>
+      <c r="I30" s="7"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="H31" s="7"/>
+        <v>104</v>
+      </c>
+      <c r="I31" s="7"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="H32" s="7"/>
+        <v>105</v>
+      </c>
+      <c r="I32" s="7"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="H33" s="7"/>
+        <v>106</v>
+      </c>
+      <c r="I33" s="7"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="H34" s="7"/>
+        <v>107</v>
+      </c>
+      <c r="I34" s="7"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="H35" s="7"/>
+        <v>108</v>
+      </c>
+      <c r="I35" s="7"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="H36" s="7"/>
+        <v>109</v>
+      </c>
+      <c r="I36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1788,10 +1793,10 @@
         <v>8</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1799,130 +1804,130 @@
         <v>8</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="H39" s="7"/>
+        <v>112</v>
+      </c>
+      <c r="I39" s="7"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="H40" s="7"/>
+        <v>113</v>
+      </c>
+      <c r="I40" s="7"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="H41" s="7"/>
+        <v>114</v>
+      </c>
+      <c r="I41" s="7"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="H42" s="7"/>
+        <v>115</v>
+      </c>
+      <c r="I42" s="7"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="H43" s="7"/>
+        <v>116</v>
+      </c>
+      <c r="I43" s="7"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="H44" s="7"/>
+        <v>117</v>
+      </c>
+      <c r="I44" s="7"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="H45" s="7"/>
+        <v>118</v>
+      </c>
+      <c r="I45" s="7"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="H46" s="7"/>
+        <v>119</v>
+      </c>
+      <c r="I46" s="7"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="H47" s="7"/>
+        <v>120</v>
+      </c>
+      <c r="I47" s="7"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="H48" s="7"/>
+        <v>121</v>
+      </c>
+      <c r="I48" s="7"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1930,10 +1935,10 @@
         <v>8</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1941,130 +1946,130 @@
         <v>8</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="H51" s="7"/>
+        <v>124</v>
+      </c>
+      <c r="I51" s="7"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="H52" s="7"/>
+        <v>125</v>
+      </c>
+      <c r="I52" s="7"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="H53" s="7"/>
+        <v>126</v>
+      </c>
+      <c r="I53" s="7"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="H54" s="7"/>
+        <v>127</v>
+      </c>
+      <c r="I54" s="7"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="H55" s="7"/>
+        <v>128</v>
+      </c>
+      <c r="I55" s="7"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="H56" s="7"/>
+        <v>129</v>
+      </c>
+      <c r="I56" s="7"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="H57" s="7"/>
+        <v>130</v>
+      </c>
+      <c r="I57" s="7"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="H58" s="7"/>
+        <v>131</v>
+      </c>
+      <c r="I58" s="7"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="H59" s="7"/>
+        <v>132</v>
+      </c>
+      <c r="I59" s="7"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="H60" s="7"/>
+        <v>133</v>
+      </c>
+      <c r="I60" s="7"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2072,31 +2077,31 @@
         <v>8</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="E62" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="F62" s="4" t="s">
+      <c r="F62" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="G62" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G62" s="0" t="n">
+      <c r="H62" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H62" s="7" t="n">
+      <c r="I62" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="I62" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="J62" s="4" t="s">
+      <c r="J62" s="0" t="s">
         <v>138</v>
+      </c>
+      <c r="K62" s="4" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2104,29 +2109,29 @@
         <v>8</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="E63" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="F63" s="4" t="s">
+      <c r="F63" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="G63" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G63" s="0" t="n">
+      <c r="H63" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="H63" s="7" t="n">
+      <c r="I63" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I63" s="0" t="s">
-        <v>137</v>
+      <c r="J63" s="0" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2134,29 +2139,29 @@
         <v>8</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="E64" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="F64" s="4" t="s">
+      <c r="F64" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="G64" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G64" s="0" t="n">
+      <c r="H64" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="H64" s="7" t="n">
+      <c r="I64" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I64" s="0" t="s">
-        <v>137</v>
+      <c r="J64" s="0" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2164,29 +2169,29 @@
         <v>8</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="E65" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="F65" s="4" t="s">
+      <c r="F65" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="G65" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G65" s="0" t="n">
+      <c r="H65" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="H65" s="7" t="n">
+      <c r="I65" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I65" s="0" t="s">
-        <v>137</v>
+      <c r="J65" s="0" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2194,29 +2199,29 @@
         <v>8</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="E66" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="F66" s="4" t="s">
+      <c r="F66" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="G66" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G66" s="0" t="n">
+      <c r="H66" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="H66" s="7" t="n">
+      <c r="I66" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I66" s="0" t="s">
-        <v>137</v>
+      <c r="J66" s="0" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2224,29 +2229,29 @@
         <v>8</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="E67" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="F67" s="4" t="s">
+      <c r="F67" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="G67" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G67" s="0" t="n">
+      <c r="H67" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="H67" s="7" t="n">
+      <c r="I67" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I67" s="0" t="s">
-        <v>137</v>
+      <c r="J67" s="0" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2254,29 +2259,29 @@
         <v>8</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="E68" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="F68" s="4" t="s">
+      <c r="F68" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="G68" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G68" s="0" t="n">
+      <c r="H68" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="H68" s="7" t="n">
+      <c r="I68" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I68" s="0" t="s">
-        <v>137</v>
+      <c r="J68" s="0" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2284,29 +2289,29 @@
         <v>8</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="E69" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="F69" s="4" t="s">
+      <c r="F69" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="G69" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G69" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="H69" s="7" t="n">
+      <c r="H69" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="I69" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I69" s="0" t="s">
-        <v>137</v>
+      <c r="J69" s="0" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2314,29 +2319,29 @@
         <v>8</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="E70" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="F70" s="4" t="s">
+      <c r="F70" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="G70" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G70" s="0" t="n">
+      <c r="H70" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="H70" s="7" t="n">
+      <c r="I70" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I70" s="0" t="s">
-        <v>137</v>
+      <c r="J70" s="0" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2344,29 +2349,29 @@
         <v>8</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="E71" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="F71" s="4" t="s">
+      <c r="F71" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="G71" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G71" s="0" t="n">
+      <c r="H71" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="H71" s="7" t="n">
+      <c r="I71" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="I71" s="0" t="s">
-        <v>137</v>
+      <c r="J71" s="0" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2374,26 +2379,26 @@
         <v>8</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="E72" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="G72" s="0" t="n">
+      <c r="F72" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="H72" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="H72" s="7" t="n">
+      <c r="I72" s="7" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I72" s="0" t="s">
-        <v>149</v>
+      <c r="J72" s="0" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2401,10 +2406,10 @@
         <v>8</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2412,10 +2417,10 @@
         <v>8</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2423,130 +2428,130 @@
         <v>8</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="H75" s="7"/>
+        <v>153</v>
+      </c>
+      <c r="I75" s="7"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="H76" s="7"/>
+        <v>154</v>
+      </c>
+      <c r="I76" s="7"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="H77" s="7"/>
+        <v>155</v>
+      </c>
+      <c r="I77" s="7"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="H78" s="7"/>
+        <v>156</v>
+      </c>
+      <c r="I78" s="7"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="H79" s="7"/>
+        <v>157</v>
+      </c>
+      <c r="I79" s="7"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="H80" s="7"/>
+        <v>158</v>
+      </c>
+      <c r="I80" s="7"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="H81" s="7"/>
+        <v>159</v>
+      </c>
+      <c r="I81" s="7"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="H82" s="7"/>
+        <v>160</v>
+      </c>
+      <c r="I82" s="7"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="H83" s="7"/>
+        <v>161</v>
+      </c>
+      <c r="I83" s="7"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="H84" s="7"/>
+        <v>162</v>
+      </c>
+      <c r="I84" s="7"/>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2554,10 +2559,10 @@
         <v>8</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2565,10 +2570,10 @@
         <v>8</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2576,10 +2581,10 @@
         <v>8</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2587,10 +2592,10 @@
         <v>8</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2598,10 +2603,10 @@
         <v>8</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2609,10 +2614,10 @@
         <v>8</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2620,10 +2625,10 @@
         <v>8</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2631,10 +2636,10 @@
         <v>8</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2642,10 +2647,10 @@
         <v>8</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2653,10 +2658,10 @@
         <v>8</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2664,10 +2669,10 @@
         <v>8</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2675,12 +2680,12 @@
         <v>8</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="H97" s="7"/>
+        <v>175</v>
+      </c>
+      <c r="I97" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2701,12 +2706,12 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="1" sqref="D1 D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="72.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.34"/>
@@ -2714,10 +2719,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>0</v>
@@ -2728,16 +2733,16 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -2756,54 +2761,51 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="D1 F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="13.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="31.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="13.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="31.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>67</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="H1" s="0" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>185</v>
@@ -2814,22 +2816,19 @@
       <c r="E2" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="F2" s="0" t="n">
-        <v>10</v>
+      <c r="F2" s="0" t="s">
+        <v>188</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="H2" s="0" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>185</v>
@@ -2840,22 +2839,19 @@
       <c r="E3" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="F3" s="0" t="n">
-        <v>10</v>
+      <c r="F3" s="0" t="s">
+        <v>190</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="H3" s="0" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>185</v>
@@ -2866,22 +2862,19 @@
       <c r="E4" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="F4" s="0" t="n">
-        <v>10</v>
+      <c r="F4" s="0" t="s">
+        <v>192</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="H4" s="0" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>185</v>
@@ -2892,22 +2885,19 @@
       <c r="E5" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="F5" s="0" t="n">
-        <v>10</v>
+      <c r="F5" s="0" t="s">
+        <v>194</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="H5" s="0" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>185</v>
@@ -2918,22 +2908,19 @@
       <c r="E6" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="F6" s="0" t="n">
-        <v>10</v>
+      <c r="F6" s="0" t="s">
+        <v>196</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="H6" s="0" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>185</v>
@@ -2944,22 +2931,19 @@
       <c r="E7" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="F7" s="0" t="n">
-        <v>10</v>
+      <c r="F7" s="0" t="s">
+        <v>198</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="H7" s="0" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>185</v>
@@ -2970,22 +2954,19 @@
       <c r="E8" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="F8" s="0" t="n">
-        <v>10</v>
+      <c r="F8" s="0" t="s">
+        <v>200</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="H8" s="0" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>185</v>
@@ -2996,22 +2977,19 @@
       <c r="E9" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="F9" s="0" t="n">
-        <v>10</v>
+      <c r="F9" s="0" t="s">
+        <v>202</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="H9" s="0" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>185</v>
@@ -3022,22 +3000,19 @@
       <c r="E10" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="F10" s="0" t="n">
-        <v>10</v>
+      <c r="F10" s="0" t="s">
+        <v>204</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>204</v>
-      </c>
-      <c r="H10" s="0" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>185</v>
@@ -3048,22 +3023,19 @@
       <c r="E11" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="F11" s="0" t="n">
-        <v>10</v>
+      <c r="F11" s="0" t="s">
+        <v>206</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>206</v>
-      </c>
-      <c r="H11" s="0" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>185</v>
@@ -3074,13 +3046,10 @@
       <c r="E12" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="F12" s="0" t="n">
-        <v>10</v>
+      <c r="F12" s="0" t="s">
+        <v>208</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="H12" s="0" t="s">
         <v>209</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add project_type in Project and calculate score to be loaded in MutationSummary as well as variant_caller_presence
</commit_message>
<xml_diff>
--- a/data/20170201_GEP00003/20170201_GEP00003.xlsx
+++ b/data/20170201_GEP00003/20170201_GEP00003.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="212">
   <si>
     <t xml:space="preserve">geid</t>
   </si>
@@ -50,6 +50,9 @@
     <t xml:space="preserve">start_date</t>
   </si>
   <si>
+    <t xml:space="preserve">project_type</t>
+  </si>
+  <si>
     <t xml:space="preserve">description</t>
   </si>
   <si>
@@ -69,6 +72,9 @@
   </si>
   <si>
     <t xml:space="preserve">Alasdair Russel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">knock-in</t>
   </si>
   <si>
     <t xml:space="preserve">eGFP Knock-in to turn it into eBFP. NGS to detect the modification in a population of cells.</t>
@@ -869,10 +875,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -882,8 +888,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="11.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="15.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="33.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="33.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -911,31 +918,37 @@
       <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>20170201</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -957,7 +970,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="1" sqref="D1 J2"/>
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -971,51 +984,51 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>23</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>0</v>
@@ -1027,10 +1040,10 @@
         <v>0</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1052,7 +1065,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="1" sqref="D1 F3"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1066,39 +1079,39 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>62</v>
@@ -1107,10 +1120,10 @@
         <v>1</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1131,7 +1144,7 @@
   </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -1139,23 +1152,23 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1177,7 +1190,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="1" sqref="D1 E3"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1204,87 +1217,87 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>202</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K2" s="0" t="n">
         <v>131</v>
@@ -1293,10 +1306,10 @@
         <v>151</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="O2" s="0" t="n">
         <v>245</v>
@@ -1305,7 +1318,7 @@
         <v>264</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1327,7 +1340,7 @@
   <dimension ref="A1:K97"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="D1 E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1344,752 +1357,752 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="I18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="I22" s="7"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="I23" s="7"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I24" s="7"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I27" s="7"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I28" s="7"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="I29" s="7"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I30" s="7"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I31" s="7"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I32" s="7"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I33" s="7"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I34" s="7"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="I35" s="7"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="I36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="I39" s="7"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="I40" s="7"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I41" s="7"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="I42" s="7"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I43" s="7"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="I44" s="7"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="I45" s="7"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="I46" s="7"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="I47" s="7"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="I48" s="7"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="I51" s="7"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="I52" s="7"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="I53" s="7"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="I54" s="7"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="I55" s="7"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I56" s="7"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="I57" s="7"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I58" s="7"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="I59" s="7"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="I60" s="7"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H62" s="0" t="n">
         <v>1</v>
@@ -2098,30 +2111,30 @@
         <v>0</v>
       </c>
       <c r="J62" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="K62" s="4" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H63" s="0" t="n">
         <v>2</v>
@@ -2131,27 +2144,27 @@
         <v>0</v>
       </c>
       <c r="J63" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H64" s="0" t="n">
         <v>3</v>
@@ -2161,27 +2174,27 @@
         <v>0</v>
       </c>
       <c r="J64" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H65" s="0" t="n">
         <v>4</v>
@@ -2191,27 +2204,27 @@
         <v>0</v>
       </c>
       <c r="J65" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H66" s="0" t="n">
         <v>5</v>
@@ -2221,27 +2234,27 @@
         <v>0</v>
       </c>
       <c r="J66" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H67" s="0" t="n">
         <v>6</v>
@@ -2251,27 +2264,27 @@
         <v>0</v>
       </c>
       <c r="J67" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H68" s="0" t="n">
         <v>7</v>
@@ -2281,27 +2294,27 @@
         <v>0</v>
       </c>
       <c r="J68" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H69" s="0" t="n">
         <v>8</v>
@@ -2311,27 +2324,27 @@
         <v>0</v>
       </c>
       <c r="J69" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H70" s="0" t="n">
         <v>9</v>
@@ -2341,27 +2354,27 @@
         <v>0</v>
       </c>
       <c r="J70" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H71" s="0" t="n">
         <v>10</v>
@@ -2371,24 +2384,24 @@
         <v>0</v>
       </c>
       <c r="J71" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="H72" s="0" t="n">
         <v>11</v>
@@ -2398,292 +2411,292 @@
         <v>1</v>
       </c>
       <c r="J72" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="I75" s="7"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="I76" s="7"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="I77" s="7"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="I78" s="7"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="I79" s="7"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I80" s="7"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="I81" s="7"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="I82" s="7"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="I83" s="7"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="I84" s="7"/>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="I97" s="7"/>
     </row>
@@ -2706,7 +2719,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="1" sqref="D1 D3"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2719,30 +2732,30 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -2764,7 +2777,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="D1 F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2779,278 +2792,278 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>